<commit_message>
Solve findMaximumCPULoad Solve print nodes at k distance in a tree
</commit_message>
<xml_diff>
--- a/EducativeIO/Documents/DS and Algos.xlsx
+++ b/EducativeIO/Documents/DS and Algos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\SWE\Educative\EducativeIO\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2686AA93-D249-40F8-AE41-05E53DD0B4E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A13A21-0BB8-469E-8C2A-EEB175BA48D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21390" xr2:uid="{33A75E95-E37D-4FE2-9DBD-2120326E4772}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15555" xr2:uid="{33A75E95-E37D-4FE2-9DBD-2120326E4772}"/>
   </bookViews>
   <sheets>
     <sheet name="Merge Intervals" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Todo</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Hard</t>
+  </si>
+  <si>
+    <t>Problem Challenge 2 - Grokking the Coding Interview: Patterns for Coding Questions (educative.io)</t>
   </si>
 </sst>
 </file>
@@ -122,7 +125,38 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -144,6 +178,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D029F68-CB28-4762-8604-2B6D7D716344}" name="Table1" displayName="Table1" ref="A1:D3" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+  <autoFilter ref="A1:D3" xr:uid="{8D029F68-CB28-4762-8604-2B6D7D716344}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E71CB30B-8E31-4EAA-9427-88FCFD4354C6}" name="Todo" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{D6F761E5-9193-4198-A077-069509F73EFA}" name="Confidence Level" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8718900D-DB0D-4E74-9D76-9EAE8B0061C4}" name="Redo?" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{722A5FB1-07E2-4671-970A-0C18CF9F05B6}" name="Level" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,17 +490,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BB86AE-8FD1-467C-A0AF-919CA6E72128}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="90.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="4"/>
+    <col min="2" max="2" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -484,16 +532,34 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="A1:D2 B3:D3">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://www.educative.io/courses/grokking-the-coding-interview/xVoBRZz7RwP" xr:uid="{10698BE1-0F9F-43BE-95FA-027FE8B9FA79}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.educative.io/courses/grokking-the-coding-interview/xVlyyv3rR93" xr:uid="{EB67C15B-7CD8-4433-B625-0282042C9547}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solve valid palindrome with deleted character
</commit_message>
<xml_diff>
--- a/EducativeIO/Documents/DS and Algos.xlsx
+++ b/EducativeIO/Documents/DS and Algos.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\SWE\Educative\EducativeIO\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A13A21-0BB8-469E-8C2A-EEB175BA48D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358BF563-4996-4B1B-B1AB-47C6725C37E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15555" xr2:uid="{33A75E95-E37D-4FE2-9DBD-2120326E4772}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21150" activeTab="1" xr2:uid="{33A75E95-E37D-4FE2-9DBD-2120326E4772}"/>
   </bookViews>
   <sheets>
     <sheet name="Merge Intervals" sheetId="1" r:id="rId1"/>
+    <sheet name="Facebook" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Todo</t>
   </si>
@@ -58,12 +59,51 @@
   </si>
   <si>
     <t>Problem Challenge 2 - Grokking the Coding Interview: Patterns for Coding Questions (educative.io)</t>
+  </si>
+  <si>
+    <t>Question Url</t>
+  </si>
+  <si>
+    <t>Solved?</t>
+  </si>
+  <si>
+    <t>How Long</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Looked at discussions</t>
+  </si>
+  <si>
+    <t>Date of Review 1</t>
+  </si>
+  <si>
+    <t>Date of Review 2</t>
+  </si>
+  <si>
+    <t>Date of Review 3</t>
+  </si>
+  <si>
+    <t>First Solution</t>
+  </si>
+  <si>
+    <t>Valid Palindrome II - LeetCode</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>2 Pointers, Loop, check if left is not equal to right, if a character is deleted, return false, else, try deleting a character by recursing through the function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -120,12 +160,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -154,19 +211,6 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -181,13 +225,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D029F68-CB28-4762-8604-2B6D7D716344}" name="Table1" displayName="Table1" ref="A1:D3" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D029F68-CB28-4762-8604-2B6D7D716344}" name="Table1" displayName="Table1" ref="A1:D3" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D3" xr:uid="{8D029F68-CB28-4762-8604-2B6D7D716344}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E71CB30B-8E31-4EAA-9427-88FCFD4354C6}" name="Todo" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{D6F761E5-9193-4198-A077-069509F73EFA}" name="Confidence Level" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{8718900D-DB0D-4E74-9D76-9EAE8B0061C4}" name="Redo?" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{722A5FB1-07E2-4671-970A-0C18CF9F05B6}" name="Level" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{D6F761E5-9193-4198-A077-069509F73EFA}" name="Confidence Level" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{8718900D-DB0D-4E74-9D76-9EAE8B0061C4}" name="Redo?" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{722A5FB1-07E2-4671-970A-0C18CF9F05B6}" name="Level" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -492,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BB86AE-8FD1-467C-A0AF-919CA6E72128}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -548,7 +592,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D2 B3:D3">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -562,4 +606,74 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4D3A04-7FDA-425C-BD71-220CA01FE33B}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="5" customWidth="1"/>
+    <col min="6" max="8" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5">
+        <v>44391</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://leetcode.com/problems/valid-palindrome-ii/" xr:uid="{F5BDFC44-76B6-4A2D-BFF0-CAC7C33176A6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>